<commit_message>
added time detail to spreadsheet
</commit_message>
<xml_diff>
--- a/Week9Project_TaskList.xlsx
+++ b/Week9Project_TaskList.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnm\Google Drive\2018-Spring\CIS-269\Week09\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnm\Google Drive\2018-Spring\CIS-269\Week09\Snake\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C620D229-D8A9-4600-A55E-50B321EF91DD}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4DA0099-91AB-485A-95B2-B38FA8B2F8AF}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
   <si>
     <t>Update snake graphic</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>45 minutes</t>
+  </si>
+  <si>
+    <t>1 minute</t>
   </si>
 </sst>
 </file>
@@ -550,8 +553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="U8" sqref="U8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -757,6 +760,9 @@
       <c r="P9" s="6"/>
       <c r="Q9" s="6"/>
       <c r="R9" s="6"/>
+      <c r="U9" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
@@ -775,6 +781,9 @@
       <c r="P10" s="6"/>
       <c r="Q10" s="6"/>
       <c r="R10" s="6"/>
+      <c r="U10" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="5">

</xml_diff>